<commit_message>
Updated Test Cases Excel Sheet
</commit_message>
<xml_diff>
--- a/TestCasesSDS.xlsx
+++ b/TestCasesSDS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F44719AC-C001-4EA6-B6F8-2A3D55454F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1651F502-D50B-4721-9E45-790551DFC0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9675" yWindow="1260" windowWidth="24105" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -201,6 +201,99 @@
   </si>
   <si>
     <t>The user interacts with the search bar, types in their wanted movie and it shows up at the top.</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Registration_Module</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>User registers with valid input and verifies email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Register 2)Enter First name = Jonah, Last name = Ale, Email = JonahisJonah@gmail.com, Username = JonahIsJonah, Password = 123sT!sl, Comfirm passwords match 3) Click "I agree to terms" 4) Click "Create an Account" </t>
+  </si>
+  <si>
+    <t>Verification services working</t>
+  </si>
+  <si>
+    <t>Account should be succefully created after validating input</t>
+  </si>
+  <si>
+    <t>Account for a new user was created</t>
+  </si>
+  <si>
+    <t>Email Validation</t>
+  </si>
+  <si>
+    <t>validateEmail(email)</t>
+  </si>
+  <si>
+    <t>Verify that the email validation inside the registratrion process is working correctly and doesn't alllow invalid email formats</t>
+  </si>
+  <si>
+    <t>Registration module is fully compiled. Email validation is fully functional.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) call validateEmail("JonahisJonah@gmail.com")  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returns "Valid" </t>
+  </si>
+  <si>
+    <t>Returns "Valid"</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>Qr Code Generator</t>
+  </si>
+  <si>
+    <t>GenerateQRCode(TicketID</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>Verify that a QR code is generated and the encoding pertains to the correct ticket.</t>
+  </si>
+  <si>
+    <t>A valid ticket was purchased</t>
+  </si>
+  <si>
+    <t>1) Call GenerateQRCode("TCBD-12345"). 2) Decode the QR code to verify it</t>
+  </si>
+  <si>
+    <t>An image of the QR code is succfully created and the decoding matches</t>
+  </si>
+  <si>
+    <t>A QR code is cuccfully created and the decoded code matches TCBD-12345</t>
+  </si>
+  <si>
+    <t>Process Payment</t>
+  </si>
+  <si>
+    <t>ProcessPayment(orderID, amount, paymentMethod)</t>
+  </si>
+  <si>
+    <t>Verify that when a payment request is made the system interacts with the payment service and returns a valid PaymentID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A valid orderID exists. </t>
+  </si>
+  <si>
+    <t>1) Call ProcessPayment(orderID="12345", amount = "15.99", paymentMethod = "Visa") 2) Verify that the PaymentID is displayed and is recorded on the order record.</t>
+  </si>
+  <si>
+    <t>The payment service return a valid PaymentID</t>
+  </si>
+  <si>
+    <t>A valid payment id</t>
   </si>
 </sst>
 </file>
@@ -264,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -287,11 +380,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -305,6 +409,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,27 +721,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -643,7 +755,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -707,7 +819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -739,7 +851,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="91.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="81" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -771,7 +883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="114" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -803,7 +915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
@@ -835,7 +947,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="114" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="103.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -865,6 +977,134 @@
       </c>
       <c r="J8" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="81" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated new Test Cases for Excel Sheet
</commit_message>
<xml_diff>
--- a/TestCasesSDS.xlsx
+++ b/TestCasesSDS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1651F502-D50B-4721-9E45-790551DFC0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7590BD-481E-43F7-B333-F99A3E4E3D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="102">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -294,6 +294,48 @@
   </si>
   <si>
     <t>A valid payment id</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>System Test01</t>
+  </si>
+  <si>
+    <t>System Test02</t>
+  </si>
+  <si>
+    <t>App is running and database can be accessed</t>
+  </si>
+  <si>
+    <t>1) Register 2) Enter valid email/password 3) Click submit.</t>
+  </si>
+  <si>
+    <t>"Successful registration" displayed and a new user is store in the database. An email verification link is sent.</t>
+  </si>
+  <si>
+    <t>Verify that a newly registered user can  activate their account with their email</t>
+  </si>
+  <si>
+    <t>User created.</t>
+  </si>
+  <si>
+    <t>1) Open verification email. 2) Cick activation link 3) Return to app and attempt to login</t>
+  </si>
+  <si>
+    <t>Account labeled as "Active". Login is successful .</t>
+  </si>
+  <si>
+    <t>The account was registered</t>
+  </si>
+  <si>
+    <t>Verify that a user can register successfully with valid credentials.</t>
+  </si>
+  <si>
+    <t>The account was activated.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -406,6 +448,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,7 +466,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,18 +791,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -980,132 +1029,208 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="81" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>72</v>
       </c>
+    </row>
+    <row r="13" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>